<commit_message>
Ajustes + Tela de Carteiras
</commit_message>
<xml_diff>
--- a/AASPA/Relatorio/RelAverbacao.202406.xlsx
+++ b/AASPA/Relatorio/RelAverbacao.202406.xlsx
@@ -9,7 +9,7 @@
     <x:sheet name="Relatório Averbacao" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="_xlnm.Print_Area" localSheetId="0">'Relatório Averbacao'!$A$1:$G$22</x:definedName>
+    <x:definedName name="_xlnm.Print_Area" localSheetId="0">'Relatório Averbacao'!$A$1:$G$19</x:definedName>
     <x:definedName name="_xlnm.Print_Titles" localSheetId="0">'Relatório Averbacao'!1:4</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="125725"/>
@@ -31,10 +31,16 @@
     <x:t>Motivos não averbados</x:t>
   </x:si>
   <x:si>
+    <x:t>Total não averbados</x:t>
+  </x:si>
+  <x:si>
+    <x:t>%</x:t>
+  </x:si>
+  <x:si>
     <x:t>CORRETORA:</x:t>
   </x:si>
   <x:si>
-    <x:t>Confia</x:t>
+    <x:t>aaspa</x:t>
   </x:si>
   <x:si>
     <x:t>002 - Espécie incompatível</x:t>
@@ -49,6 +55,9 @@
     <x:t>004 - NB inexistente no cadastro</x:t>
   </x:si>
   <x:si>
+    <x:t>100%</x:t>
+  </x:si>
+  <x:si>
     <x:t>Averbados:</x:t>
   </x:si>
   <x:si>
@@ -58,7 +67,7 @@
     <x:t>Taxa de Averbação:</x:t>
   </x:si>
   <x:si>
-    <x:t>100%</x:t>
+    <x:t>33%</x:t>
   </x:si>
   <x:si>
     <x:t>006 - Valor ultrapassa MR do titular</x:t>
@@ -67,12 +76,18 @@
     <x:t>008 - Já existe desc. p/ outra entidade</x:t>
   </x:si>
   <x:si>
+    <x:t>0</x:t>
+  </x:si>
+  <x:si>
     <x:t>012 - Benefício bloqueado para desconto</x:t>
   </x:si>
   <x:si>
     <x:t>Total Não averbado</x:t>
   </x:si>
   <x:si>
+    <x:t>66%</x:t>
+  </x:si>
+  <x:si>
     <x:t>Detalhe de Produção</x:t>
   </x:si>
   <x:si>
@@ -97,31 +112,25 @@
     <x:t>Motivo</x:t>
   </x:si>
   <x:si>
-    <x:t>1599678931</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Luana Sofia Rodrigues Silva</x:t>
+    <x:t>ADRIANO PAULO FERREIRA DA SILVA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Não Averbado</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NB inexistente no cadastro</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DIRCE BENTO DA SILVA</x:t>
   </x:si>
   <x:si>
     <x:t>Averbado</x:t>
   </x:si>
   <x:si>
-    <x:t>(OK) Consignação incluída</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1556939245</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Joao Da Silva</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1478292307</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Teste Cliente</x:t>
-  </x:si>
-  <x:si>
     <x:t>(OK) Consignação excluída</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EDIS DEMORI</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -442,6 +451,42 @@
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
 </x:styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2200275" cy="762000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2200275" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect"/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -732,7 +777,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G22"/>
+  <x:dimension ref="A1:G19"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -741,8 +786,7 @@
     <x:col min="1" max="1" width="18.710625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="15.710625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="40.710625" style="0" customWidth="1"/>
-    <x:col min="4" max="5" width="15.710625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="18.710625" style="0" customWidth="1"/>
+    <x:col min="4" max="6" width="18.710625" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="38.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
@@ -800,288 +844,223 @@
       <x:c r="D6" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="F6" s="10"/>
-      <x:c r="G6" s="11"/>
+      <x:c r="F6" s="10" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="G6" s="11" t="s">
+        <x:v>5</x:v>
+      </x:c>
     </x:row>
     <x:row r="7" spans="1:7">
       <x:c r="A7" s="9" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F7" s="10">
         <x:v>0</x:v>
       </x:c>
       <x:c r="G7" s="11" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:7">
       <x:c r="A8" s="9" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B8" s="0">
         <x:v>3</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="F8" s="10">
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="G8" s="11" t="s">
-        <x:v>7</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:7">
       <x:c r="A9" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B9" s="0">
-        <x:v>3</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="F9" s="10">
         <x:v>0</x:v>
       </x:c>
       <x:c r="G9" s="11" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:7">
       <x:c r="A10" s="9" t="s">
-        <x:v>12</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F10" s="10">
         <x:v>0</x:v>
       </x:c>
       <x:c r="G10" s="11" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:7">
       <x:c r="A11" s="9"/>
       <x:c r="D11" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F11" s="10">
         <x:v>0</x:v>
       </x:c>
       <x:c r="G11" s="11" t="s">
-        <x:v>7</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:7">
       <x:c r="A12" s="9"/>
       <x:c r="D12" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F12" s="10">
-        <x:v>0</x:v>
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F12" s="10" t="s">
+        <x:v>19</x:v>
       </x:c>
       <x:c r="G12" s="11" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:7">
       <x:c r="A13" s="9"/>
       <x:c r="D13" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F13" s="10">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="G13" s="11" t="s">
-        <x:v>7</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:7">
       <x:c r="A14" s="7" t="s">
-        <x:v>18</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="G14" s="8"/>
     </x:row>
     <x:row r="15" spans="1:7">
       <x:c r="A15" s="12" t="s">
-        <x:v>19</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B15" s="10" t="s">
-        <x:v>20</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C15" s="10" t="s">
-        <x:v>21</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D15" s="10" t="s">
-        <x:v>22</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E15" s="10" t="s">
-        <x:v>23</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F15" s="10" t="s">
-        <x:v>24</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G15" s="11" t="s">
-        <x:v>25</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:7">
-      <x:c r="A16" s="12" t="s">
-        <x:v>26</x:v>
+      <x:c r="A16" s="12">
+        <x:v>1983384280</x:v>
       </x:c>
       <x:c r="B16" s="10">
-        <x:v>16774562647</x:v>
+        <x:v>84786949434</x:v>
       </x:c>
       <x:c r="C16" s="10" t="s">
-        <x:v>27</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D16" s="13">
-        <x:v>45413</x:v>
+        <x:v>45465</x:v>
       </x:c>
       <x:c r="E16" s="10">
-        <x:v>7060</x:v>
+        <x:v>500</x:v>
       </x:c>
       <x:c r="F16" s="10" t="s">
-        <x:v>28</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G16" s="11" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:7">
-      <x:c r="A17" s="12" t="s">
-        <x:v>30</x:v>
+      <x:c r="A17" s="12">
+        <x:v>1547030264</x:v>
       </x:c>
       <x:c r="B17" s="10">
-        <x:v>39649346074</x:v>
+        <x:v>9239848878</x:v>
       </x:c>
       <x:c r="C17" s="10" t="s">
-        <x:v>31</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D17" s="13">
-        <x:v>45461</x:v>
+        <x:v>45465</x:v>
       </x:c>
       <x:c r="E17" s="10">
-        <x:v>0</x:v>
+        <x:v>500</x:v>
       </x:c>
       <x:c r="F17" s="10" t="s">
-        <x:v>28</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="G17" s="11" t="s">
-        <x:v>29</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:7">
-      <x:c r="A18" s="12" t="s">
+      <x:c r="A18" s="12">
+        <x:v>2225096524</x:v>
+      </x:c>
+      <x:c r="B18" s="10">
+        <x:v>1023044838</x:v>
+      </x:c>
+      <x:c r="C18" s="10" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="D18" s="13">
+        <x:v>45465</x:v>
+      </x:c>
+      <x:c r="E18" s="10">
+        <x:v>500</x:v>
+      </x:c>
+      <x:c r="F18" s="10" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="B18" s="10">
-        <x:v>16041605603</x:v>
-      </x:c>
-      <x:c r="C18" s="10" t="s">
+      <x:c r="G18" s="11" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="D18" s="13">
-        <x:v>45413</x:v>
-      </x:c>
-      <x:c r="E18" s="10">
-        <x:v>7786</x:v>
-      </x:c>
-      <x:c r="F18" s="10" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="G18" s="11" t="s">
-        <x:v>29</x:v>
-      </x:c>
     </x:row>
     <x:row r="19" spans="1:7">
-      <x:c r="A19" s="12" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="B19" s="10">
-        <x:v>16774562647</x:v>
-      </x:c>
-      <x:c r="C19" s="10" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="D19" s="13">
-        <x:v>45413</x:v>
-      </x:c>
-      <x:c r="E19" s="10">
-        <x:v>7060</x:v>
-      </x:c>
-      <x:c r="F19" s="10" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="G19" s="11" t="s">
-        <x:v>34</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:7">
-      <x:c r="A20" s="12" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="B20" s="10">
-        <x:v>39649346074</x:v>
-      </x:c>
-      <x:c r="C20" s="10" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="D20" s="13">
-        <x:v>45461</x:v>
-      </x:c>
-      <x:c r="E20" s="10">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F20" s="10" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="G20" s="11" t="s">
-        <x:v>34</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:7">
-      <x:c r="A21" s="12" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="B21" s="10">
-        <x:v>16041605603</x:v>
-      </x:c>
-      <x:c r="C21" s="10" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="D21" s="13">
-        <x:v>45413</x:v>
-      </x:c>
-      <x:c r="E21" s="10">
-        <x:v>7786</x:v>
-      </x:c>
-      <x:c r="F21" s="10" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="G21" s="11" t="s">
-        <x:v>34</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:7">
-      <x:c r="A22" s="14"/>
-      <x:c r="B22" s="15"/>
-      <x:c r="C22" s="15"/>
-      <x:c r="D22" s="15"/>
-      <x:c r="E22" s="15"/>
-      <x:c r="F22" s="15"/>
-      <x:c r="G22" s="16"/>
+      <x:c r="A19" s="14"/>
+      <x:c r="B19" s="15"/>
+      <x:c r="C19" s="15"/>
+      <x:c r="D19" s="15"/>
+      <x:c r="E19" s="15"/>
+      <x:c r="F19" s="15"/>
+      <x:c r="G19" s="16"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="3">
@@ -1093,6 +1072,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="landscape" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
+  <x:drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
</xml_diff>